<commit_message>
Removal of old storyboard files
</commit_message>
<xml_diff>
--- a/_doc/WARC Portal.xlsx
+++ b/_doc/WARC Portal.xlsx
@@ -5,11 +5,11 @@
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrianomarini/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrianomarini/Desktop/WARC-Portal/_doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="920" yWindow="440" windowWidth="27880" windowHeight="17560"/>
+    <workbookView xWindow="940" yWindow="440" windowWidth="27860" windowHeight="17560"/>
   </bookViews>
   <sheets>
     <sheet name="GANTT" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="90">
   <si>
     <t>Plan</t>
   </si>
@@ -203,9 +203,6 @@
     <t>Design Document</t>
   </si>
   <si>
-    <t>Adriano, Mate</t>
-  </si>
-  <si>
     <t>Image extraction</t>
   </si>
   <si>
@@ -227,15 +224,6 @@
     <t>Term frequency graph</t>
   </si>
   <si>
-    <t>MySQL Database</t>
-  </si>
-  <si>
-    <t>Front End App Shell</t>
-  </si>
-  <si>
-    <t>Backend App Shell</t>
-  </si>
-  <si>
     <t>Adriano</t>
   </si>
   <si>
@@ -329,9 +317,6 @@
     <t>Mate</t>
   </si>
   <si>
-    <t>Adriano, Kevin</t>
-  </si>
-  <si>
     <t>1,4</t>
   </si>
   <si>
@@ -378,6 +363,18 @@
   </si>
   <si>
     <t>29,30,31,32</t>
+  </si>
+  <si>
+    <t>Front End App Skeleton</t>
+  </si>
+  <si>
+    <t>Backend App Skeleton</t>
+  </si>
+  <si>
+    <t>MySQL Install</t>
+  </si>
+  <si>
+    <t>Cheng + Adriano</t>
   </si>
 </sst>
 </file>
@@ -731,14 +728,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="10" fillId="0" borderId="7" xfId="3" applyBorder="1">
       <alignment horizontal="center"/>
@@ -746,17 +737,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="8" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="9" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="8" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -775,6 +760,18 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="9" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -1244,14 +1241,14 @@
   <dimension ref="A2:CG50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
     <col min="2" max="2" width="34" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18" style="2" customWidth="1"/>
     <col min="4" max="4" width="15.83203125" style="2" customWidth="1"/>
     <col min="5" max="7" width="7.1640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="8.33203125" style="1" customWidth="1"/>
@@ -1264,26 +1261,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:85" ht="15" x14ac:dyDescent="0.2">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
     </row>
     <row r="3" spans="1:85" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
       <c r="K3" s="8" t="s">
         <v>13</v>
       </c>
@@ -1323,14 +1320,14 @@
       <c r="AR3"/>
     </row>
     <row r="4" spans="1:85" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
       <c r="BR4" s="1"/>
       <c r="BS4" s="1"/>
       <c r="BT4" s="1"/>
@@ -1373,7 +1370,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>14</v>
@@ -1424,7 +1421,7 @@
       <c r="O8" s="3">
         <v>5</v>
       </c>
-      <c r="P8" s="22">
+      <c r="P8" s="20">
         <v>6</v>
       </c>
       <c r="Q8" s="3">
@@ -1490,7 +1487,7 @@
       <c r="AK8" s="3">
         <v>27</v>
       </c>
-      <c r="AL8" s="22">
+      <c r="AL8" s="20">
         <v>28</v>
       </c>
       <c r="AM8" s="3">
@@ -1544,7 +1541,7 @@
       <c r="BC8" s="3">
         <v>45</v>
       </c>
-      <c r="BD8" s="22">
+      <c r="BD8" s="20">
         <v>46</v>
       </c>
       <c r="BE8" s="3">
@@ -1595,7 +1592,7 @@
       <c r="BT8" s="3">
         <v>62</v>
       </c>
-      <c r="BU8" s="22">
+      <c r="BU8" s="20">
         <v>63</v>
       </c>
       <c r="BV8" s="3">
@@ -1628,23 +1625,23 @@
       <c r="CE8" s="3">
         <v>73</v>
       </c>
-      <c r="CF8" s="22">
+      <c r="CF8" s="20">
         <v>74</v>
       </c>
       <c r="CG8" s="1"/>
     </row>
     <row r="9" spans="1:85" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
       <c r="K9" s="3">
         <v>21</v>
       </c>
@@ -1660,7 +1657,7 @@
       <c r="O9" s="3">
         <v>25</v>
       </c>
-      <c r="P9" s="22">
+      <c r="P9" s="20">
         <v>26</v>
       </c>
       <c r="Q9" s="3">
@@ -1726,7 +1723,7 @@
       <c r="AK9" s="3">
         <v>16</v>
       </c>
-      <c r="AL9" s="22">
+      <c r="AL9" s="20">
         <v>17</v>
       </c>
       <c r="AM9" s="3">
@@ -1780,7 +1777,7 @@
       <c r="BC9" s="3">
         <v>3</v>
       </c>
-      <c r="BD9" s="22">
+      <c r="BD9" s="20">
         <v>4</v>
       </c>
       <c r="BE9" s="3">
@@ -1831,7 +1828,7 @@
       <c r="BT9" s="3">
         <v>20</v>
       </c>
-      <c r="BU9" s="22">
+      <c r="BU9" s="20">
         <v>21</v>
       </c>
       <c r="BV9" s="3">
@@ -1864,7 +1861,7 @@
       <c r="CE9" s="3">
         <v>1</v>
       </c>
-      <c r="CF9" s="22">
+      <c r="CF9" s="20">
         <v>2</v>
       </c>
       <c r="CG9" s="1"/>
@@ -1874,11 +1871,11 @@
         <v>1</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E10" s="16">
         <v>1</v>
@@ -1895,22 +1892,22 @@
       <c r="I10" s="17">
         <v>0.8</v>
       </c>
-      <c r="P10" s="23"/>
-      <c r="AL10" s="23"/>
-      <c r="BD10" s="20"/>
-      <c r="BU10" s="20"/>
-      <c r="CF10" s="20"/>
+      <c r="P10" s="21"/>
+      <c r="AL10" s="21"/>
+      <c r="BD10" s="19"/>
+      <c r="BU10" s="19"/>
+      <c r="CF10" s="19"/>
     </row>
     <row r="11" spans="1:85" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E11" s="16">
         <v>1</v>
@@ -1927,24 +1924,24 @@
       <c r="I11" s="17">
         <v>1</v>
       </c>
-      <c r="P11" s="23"/>
-      <c r="AL11" s="23"/>
-      <c r="BD11" s="20"/>
-      <c r="BU11" s="20"/>
-      <c r="CF11" s="20"/>
+      <c r="P11" s="21"/>
+      <c r="AL11" s="21"/>
+      <c r="BD11" s="19"/>
+      <c r="BU11" s="19"/>
+      <c r="CF11" s="19"/>
     </row>
     <row r="12" spans="1:85" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>3</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E12" s="16">
         <v>1</v>
@@ -1961,11 +1958,11 @@
       <c r="I12" s="17">
         <v>1</v>
       </c>
-      <c r="P12" s="23"/>
-      <c r="AL12" s="23"/>
-      <c r="BD12" s="20"/>
-      <c r="BU12" s="20"/>
-      <c r="CF12" s="20"/>
+      <c r="P12" s="21"/>
+      <c r="AL12" s="21"/>
+      <c r="BD12" s="19"/>
+      <c r="BU12" s="19"/>
+      <c r="CF12" s="19"/>
     </row>
     <row r="13" spans="1:85" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -1978,7 +1975,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E13" s="16">
         <v>1</v>
@@ -1995,22 +1992,22 @@
       <c r="I13" s="17">
         <v>0.8</v>
       </c>
-      <c r="P13" s="23"/>
-      <c r="AL13" s="23"/>
-      <c r="BD13" s="20"/>
-      <c r="BU13" s="20"/>
-      <c r="CF13" s="20"/>
+      <c r="P13" s="21"/>
+      <c r="AL13" s="21"/>
+      <c r="BD13" s="19"/>
+      <c r="BU13" s="19"/>
+      <c r="CF13" s="19"/>
     </row>
     <row r="14" spans="1:85" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>5</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E14" s="16">
         <v>1</v>
@@ -2027,131 +2024,131 @@
       <c r="I14" s="17">
         <v>1</v>
       </c>
-      <c r="P14" s="23"/>
-      <c r="AL14" s="23"/>
-      <c r="BD14" s="20"/>
-      <c r="BU14" s="20"/>
-      <c r="CF14" s="20"/>
+      <c r="P14" s="21"/>
+      <c r="AL14" s="21"/>
+      <c r="BD14" s="19"/>
+      <c r="BU14" s="19"/>
+      <c r="CF14" s="19"/>
     </row>
     <row r="15" spans="1:85" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>6</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E15" s="16">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F15" s="16">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
       <c r="I15" s="17">
         <v>0</v>
       </c>
-      <c r="P15" s="23"/>
-      <c r="AL15" s="23"/>
-      <c r="BD15" s="20"/>
-      <c r="BU15" s="20"/>
-      <c r="CF15" s="20"/>
+      <c r="P15" s="21"/>
+      <c r="AL15" s="21"/>
+      <c r="BD15" s="19"/>
+      <c r="BU15" s="19"/>
+      <c r="CF15" s="19"/>
     </row>
     <row r="16" spans="1:85" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>7</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E16" s="16">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F16" s="16">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G16" s="16"/>
       <c r="H16" s="16"/>
       <c r="I16" s="17">
         <v>0</v>
       </c>
-      <c r="P16" s="23"/>
-      <c r="AL16" s="23"/>
-      <c r="BD16" s="20"/>
-      <c r="BU16" s="20"/>
-      <c r="CF16" s="20"/>
+      <c r="P16" s="21"/>
+      <c r="AL16" s="21"/>
+      <c r="BD16" s="19"/>
+      <c r="BU16" s="19"/>
+      <c r="CF16" s="19"/>
     </row>
     <row r="17" spans="1:84" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>8</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E17" s="16">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F17" s="16">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G17" s="16"/>
       <c r="H17" s="16"/>
       <c r="I17" s="17">
         <v>0</v>
       </c>
-      <c r="P17" s="23"/>
-      <c r="AL17" s="23"/>
-      <c r="BD17" s="20"/>
-      <c r="BU17" s="20"/>
-      <c r="CF17" s="20"/>
+      <c r="P17" s="21"/>
+      <c r="AL17" s="21"/>
+      <c r="BD17" s="19"/>
+      <c r="BU17" s="19"/>
+      <c r="CF17" s="19"/>
     </row>
     <row r="18" spans="1:84" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>9</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E18" s="16">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F18" s="16">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G18" s="16"/>
       <c r="H18" s="16"/>
       <c r="I18" s="17">
         <v>0</v>
       </c>
-      <c r="P18" s="23"/>
-      <c r="AL18" s="23"/>
-      <c r="BD18" s="20"/>
-      <c r="BU18" s="20"/>
-      <c r="CF18" s="20"/>
+      <c r="P18" s="21"/>
+      <c r="AL18" s="21"/>
+      <c r="BD18" s="19"/>
+      <c r="BU18" s="19"/>
+      <c r="CF18" s="19"/>
     </row>
     <row r="19" spans="1:84" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19">
@@ -2161,27 +2158,27 @@
         <v>30</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E19" s="16">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F19" s="16">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G19" s="16"/>
       <c r="H19" s="16"/>
       <c r="I19" s="17">
         <v>0</v>
       </c>
-      <c r="P19" s="23"/>
-      <c r="AL19" s="23"/>
-      <c r="BD19" s="20"/>
-      <c r="BU19" s="20"/>
-      <c r="CF19" s="20"/>
+      <c r="P19" s="21"/>
+      <c r="AL19" s="21"/>
+      <c r="BD19" s="19"/>
+      <c r="BU19" s="19"/>
+      <c r="CF19" s="19"/>
     </row>
     <row r="20" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20">
@@ -2191,73 +2188,73 @@
         <v>31</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E20" s="16">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F20" s="16">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G20" s="16"/>
       <c r="H20" s="16"/>
       <c r="I20" s="17">
         <v>0</v>
       </c>
-      <c r="P20" s="23"/>
-      <c r="AL20" s="23"/>
-      <c r="BD20" s="20"/>
-      <c r="BU20" s="20"/>
-      <c r="CF20" s="20"/>
+      <c r="P20" s="21"/>
+      <c r="AL20" s="21"/>
+      <c r="BD20" s="19"/>
+      <c r="BU20" s="19"/>
+      <c r="CF20" s="19"/>
     </row>
     <row r="21" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>12</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E21" s="16">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F21" s="16">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G21" s="16"/>
       <c r="H21" s="16"/>
       <c r="I21" s="17">
         <v>0</v>
       </c>
-      <c r="P21" s="23"/>
-      <c r="AL21" s="23"/>
-      <c r="BD21" s="20"/>
-      <c r="BU21" s="20"/>
-      <c r="CF21" s="20"/>
+      <c r="P21" s="21"/>
+      <c r="AL21" s="21"/>
+      <c r="BD21" s="19"/>
+      <c r="BU21" s="19"/>
+      <c r="CF21" s="19"/>
     </row>
     <row r="22" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>13</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C22" s="15">
         <v>3</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E22" s="16">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="F22" s="16">
         <v>1</v>
@@ -2267,54 +2264,54 @@
       <c r="I22" s="17">
         <v>0</v>
       </c>
-      <c r="P22" s="23"/>
-      <c r="AL22" s="23"/>
-      <c r="BD22" s="20"/>
-      <c r="BU22" s="20"/>
-      <c r="CF22" s="20"/>
+      <c r="P22" s="21"/>
+      <c r="AL22" s="21"/>
+      <c r="BD22" s="19"/>
+      <c r="BU22" s="19"/>
+      <c r="CF22" s="19"/>
     </row>
     <row r="23" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>14</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" s="33" t="s">
-        <v>82</v>
+        <v>55</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>77</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E23" s="16">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F23" s="16">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G23" s="16"/>
       <c r="H23" s="16"/>
       <c r="I23" s="17">
         <v>0</v>
       </c>
-      <c r="P23" s="23"/>
-      <c r="AL23" s="23"/>
-      <c r="BD23" s="20"/>
-      <c r="BU23" s="20"/>
-      <c r="CF23" s="20"/>
+      <c r="P23" s="21"/>
+      <c r="AL23" s="21"/>
+      <c r="BD23" s="19"/>
+      <c r="BU23" s="19"/>
+      <c r="CF23" s="19"/>
     </row>
     <row r="24" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>15</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E24" s="16">
         <v>14</v>
@@ -2327,24 +2324,24 @@
       <c r="I24" s="17">
         <v>0</v>
       </c>
-      <c r="P24" s="23"/>
-      <c r="AL24" s="23"/>
-      <c r="BD24" s="20"/>
-      <c r="BU24" s="20"/>
-      <c r="CF24" s="20"/>
+      <c r="P24" s="21"/>
+      <c r="AL24" s="21"/>
+      <c r="BD24" s="19"/>
+      <c r="BU24" s="19"/>
+      <c r="CF24" s="19"/>
     </row>
     <row r="25" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>16</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E25" s="16">
         <v>14</v>
@@ -2357,24 +2354,24 @@
       <c r="I25" s="17">
         <v>0</v>
       </c>
-      <c r="P25" s="23"/>
-      <c r="AL25" s="23"/>
-      <c r="BD25" s="20"/>
-      <c r="BU25" s="20"/>
-      <c r="CF25" s="20"/>
+      <c r="P25" s="21"/>
+      <c r="AL25" s="21"/>
+      <c r="BD25" s="19"/>
+      <c r="BU25" s="19"/>
+      <c r="CF25" s="19"/>
     </row>
     <row r="26" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>17</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E26" s="16">
         <v>14</v>
@@ -2387,24 +2384,24 @@
       <c r="I26" s="17">
         <v>0</v>
       </c>
-      <c r="P26" s="23"/>
-      <c r="AL26" s="23"/>
-      <c r="BD26" s="20"/>
-      <c r="BU26" s="20"/>
-      <c r="CF26" s="20"/>
+      <c r="P26" s="21"/>
+      <c r="AL26" s="21"/>
+      <c r="BD26" s="19"/>
+      <c r="BU26" s="19"/>
+      <c r="CF26" s="19"/>
     </row>
     <row r="27" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>18</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E27" s="16">
         <v>14</v>
@@ -2417,24 +2414,24 @@
       <c r="I27" s="17">
         <v>0</v>
       </c>
-      <c r="P27" s="23"/>
-      <c r="AL27" s="23"/>
-      <c r="BD27" s="20"/>
-      <c r="BU27" s="20"/>
-      <c r="CF27" s="20"/>
+      <c r="P27" s="21"/>
+      <c r="AL27" s="21"/>
+      <c r="BD27" s="19"/>
+      <c r="BU27" s="19"/>
+      <c r="CF27" s="19"/>
     </row>
     <row r="28" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>19</v>
       </c>
       <c r="B28" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="15" t="s">
         <v>68</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>72</v>
       </c>
       <c r="E28" s="16">
         <v>14</v>
@@ -2447,24 +2444,24 @@
       <c r="I28" s="17">
         <v>0</v>
       </c>
-      <c r="P28" s="23"/>
-      <c r="AL28" s="23"/>
-      <c r="BD28" s="20"/>
-      <c r="BU28" s="20"/>
-      <c r="CF28" s="20"/>
+      <c r="P28" s="21"/>
+      <c r="AL28" s="21"/>
+      <c r="BD28" s="19"/>
+      <c r="BU28" s="19"/>
+      <c r="CF28" s="19"/>
     </row>
     <row r="29" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>20</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E29" s="16">
         <v>14</v>
@@ -2477,24 +2474,24 @@
       <c r="I29" s="17">
         <v>0</v>
       </c>
-      <c r="P29" s="23"/>
-      <c r="AL29" s="23"/>
-      <c r="BD29" s="20"/>
-      <c r="BU29" s="20"/>
-      <c r="CF29" s="20"/>
+      <c r="P29" s="21"/>
+      <c r="AL29" s="21"/>
+      <c r="BD29" s="19"/>
+      <c r="BU29" s="19"/>
+      <c r="CF29" s="19"/>
     </row>
     <row r="30" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>21</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E30" s="16">
         <v>14</v>
@@ -2507,24 +2504,24 @@
       <c r="I30" s="17">
         <v>0</v>
       </c>
-      <c r="P30" s="23"/>
-      <c r="AL30" s="23"/>
-      <c r="BD30" s="20"/>
-      <c r="BU30" s="20"/>
-      <c r="CF30" s="20"/>
+      <c r="P30" s="21"/>
+      <c r="AL30" s="21"/>
+      <c r="BD30" s="19"/>
+      <c r="BU30" s="19"/>
+      <c r="CF30" s="19"/>
     </row>
     <row r="31" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>22</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E31" s="16">
         <v>14</v>
@@ -2537,24 +2534,24 @@
       <c r="I31" s="17">
         <v>0</v>
       </c>
-      <c r="P31" s="23"/>
-      <c r="AL31" s="23"/>
-      <c r="BD31" s="20"/>
-      <c r="BU31" s="20"/>
-      <c r="CF31" s="20"/>
+      <c r="P31" s="21"/>
+      <c r="AL31" s="21"/>
+      <c r="BD31" s="19"/>
+      <c r="BU31" s="19"/>
+      <c r="CF31" s="19"/>
     </row>
     <row r="32" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>23</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E32" s="16">
         <v>14</v>
@@ -2564,25 +2561,27 @@
       </c>
       <c r="G32" s="16"/>
       <c r="H32" s="16"/>
-      <c r="I32" s="17"/>
-      <c r="P32" s="23"/>
-      <c r="AL32" s="23"/>
-      <c r="BD32" s="20"/>
-      <c r="BU32" s="20"/>
-      <c r="CF32" s="20"/>
+      <c r="I32" s="17">
+        <v>0</v>
+      </c>
+      <c r="P32" s="21"/>
+      <c r="AL32" s="21"/>
+      <c r="BD32" s="19"/>
+      <c r="BU32" s="19"/>
+      <c r="CF32" s="19"/>
     </row>
     <row r="33" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>24</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E33" s="16">
         <v>14</v>
@@ -2592,25 +2591,27 @@
       </c>
       <c r="G33" s="16"/>
       <c r="H33" s="16"/>
-      <c r="I33" s="17"/>
-      <c r="P33" s="23"/>
-      <c r="AL33" s="23"/>
-      <c r="BD33" s="20"/>
-      <c r="BU33" s="20"/>
-      <c r="CF33" s="20"/>
+      <c r="I33" s="17">
+        <v>0</v>
+      </c>
+      <c r="P33" s="21"/>
+      <c r="AL33" s="21"/>
+      <c r="BD33" s="19"/>
+      <c r="BU33" s="19"/>
+      <c r="CF33" s="19"/>
     </row>
     <row r="34" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>25</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E34" s="16">
         <v>14</v>
@@ -2620,25 +2621,27 @@
       </c>
       <c r="G34" s="16"/>
       <c r="H34" s="16"/>
-      <c r="I34" s="17"/>
-      <c r="P34" s="23"/>
-      <c r="AL34" s="23"/>
-      <c r="BD34" s="20"/>
-      <c r="BU34" s="20"/>
-      <c r="CF34" s="20"/>
+      <c r="I34" s="17">
+        <v>0</v>
+      </c>
+      <c r="P34" s="21"/>
+      <c r="AL34" s="21"/>
+      <c r="BD34" s="19"/>
+      <c r="BU34" s="19"/>
+      <c r="CF34" s="19"/>
     </row>
     <row r="35" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>26</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E35" s="16">
         <v>14</v>
@@ -2648,23 +2651,25 @@
       </c>
       <c r="G35" s="16"/>
       <c r="H35" s="16"/>
-      <c r="I35" s="17"/>
-      <c r="P35" s="23"/>
-      <c r="AL35" s="23"/>
-      <c r="BD35" s="20"/>
-      <c r="BU35" s="20"/>
-      <c r="CF35" s="20"/>
+      <c r="I35" s="17">
+        <v>0</v>
+      </c>
+      <c r="P35" s="21"/>
+      <c r="AL35" s="21"/>
+      <c r="BD35" s="19"/>
+      <c r="BU35" s="19"/>
+      <c r="CF35" s="19"/>
     </row>
     <row r="36" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>27</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C36" s="15"/>
       <c r="D36" s="15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E36" s="16">
         <v>7</v>
@@ -2679,24 +2684,24 @@
         <v>4</v>
       </c>
       <c r="I36" s="17">
-        <v>0.8</v>
-      </c>
-      <c r="P36" s="23"/>
-      <c r="AL36" s="23"/>
-      <c r="BD36" s="20"/>
-      <c r="BU36" s="20"/>
-      <c r="CF36" s="20"/>
+        <v>1</v>
+      </c>
+      <c r="P36" s="21"/>
+      <c r="AL36" s="21"/>
+      <c r="BD36" s="19"/>
+      <c r="BU36" s="19"/>
+      <c r="CF36" s="19"/>
     </row>
     <row r="37" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>28</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C37" s="15"/>
       <c r="D37" s="15" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="E37" s="16">
         <v>7</v>
@@ -2709,24 +2714,24 @@
       <c r="I37" s="17">
         <v>0</v>
       </c>
-      <c r="P37" s="23"/>
-      <c r="AL37" s="23"/>
-      <c r="BD37" s="20"/>
-      <c r="BU37" s="20"/>
-      <c r="CF37" s="20"/>
+      <c r="P37" s="21"/>
+      <c r="AL37" s="21"/>
+      <c r="BD37" s="19"/>
+      <c r="BU37" s="19"/>
+      <c r="CF37" s="19"/>
     </row>
     <row r="38" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>29</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="E38" s="16">
         <v>22</v>
@@ -2734,29 +2739,33 @@
       <c r="F38" s="16">
         <v>53</v>
       </c>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
+      <c r="G38" s="16">
+        <v>12</v>
+      </c>
+      <c r="H38" s="16">
+        <v>4</v>
+      </c>
       <c r="I38" s="17">
-        <v>0</v>
-      </c>
-      <c r="P38" s="23"/>
-      <c r="AL38" s="23"/>
-      <c r="BD38" s="20"/>
-      <c r="BU38" s="20"/>
-      <c r="CF38" s="20"/>
+        <v>1</v>
+      </c>
+      <c r="P38" s="21"/>
+      <c r="AL38" s="21"/>
+      <c r="BD38" s="19"/>
+      <c r="BU38" s="19"/>
+      <c r="CF38" s="19"/>
     </row>
     <row r="39" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>30</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="E39" s="16">
         <v>22</v>
@@ -2764,29 +2773,33 @@
       <c r="F39" s="16">
         <v>53</v>
       </c>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
+      <c r="G39" s="16">
+        <v>12</v>
+      </c>
+      <c r="H39" s="16">
+        <v>4</v>
+      </c>
       <c r="I39" s="17">
-        <v>0</v>
-      </c>
-      <c r="P39" s="23"/>
-      <c r="AL39" s="23"/>
-      <c r="BD39" s="20"/>
-      <c r="BU39" s="20"/>
-      <c r="CF39" s="20"/>
+        <v>1</v>
+      </c>
+      <c r="P39" s="21"/>
+      <c r="AL39" s="21"/>
+      <c r="BD39" s="19"/>
+      <c r="BU39" s="19"/>
+      <c r="CF39" s="19"/>
     </row>
     <row r="40" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>31</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="E40" s="16">
         <v>22</v>
@@ -2794,26 +2807,30 @@
       <c r="F40" s="16">
         <v>53</v>
       </c>
-      <c r="G40" s="16"/>
-      <c r="H40" s="16"/>
+      <c r="G40" s="16">
+        <v>12</v>
+      </c>
+      <c r="H40" s="16">
+        <v>4</v>
+      </c>
       <c r="I40" s="17">
-        <v>0</v>
-      </c>
-      <c r="P40" s="23"/>
-      <c r="AL40" s="23"/>
-      <c r="BD40" s="20"/>
-      <c r="BU40" s="20"/>
-      <c r="CF40" s="20"/>
+        <v>1</v>
+      </c>
+      <c r="P40" s="21"/>
+      <c r="AL40" s="21"/>
+      <c r="BD40" s="19"/>
+      <c r="BU40" s="19"/>
+      <c r="CF40" s="19"/>
     </row>
     <row r="41" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>32</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C41" s="33" t="s">
-        <v>89</v>
+        <v>40</v>
+      </c>
+      <c r="C41" s="29" t="s">
+        <v>84</v>
       </c>
       <c r="D41" s="15" t="s">
         <v>29</v>
@@ -2829,21 +2846,21 @@
       <c r="I41" s="17">
         <v>0</v>
       </c>
-      <c r="P41" s="23"/>
-      <c r="AL41" s="23"/>
-      <c r="BD41" s="20"/>
-      <c r="BU41" s="20"/>
-      <c r="CF41" s="20"/>
+      <c r="P41" s="21"/>
+      <c r="AL41" s="21"/>
+      <c r="BD41" s="19"/>
+      <c r="BU41" s="19"/>
+      <c r="CF41" s="19"/>
     </row>
     <row r="42" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>33</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C42" s="33" t="s">
-        <v>90</v>
+        <v>32</v>
+      </c>
+      <c r="C42" s="29" t="s">
+        <v>85</v>
       </c>
       <c r="D42" s="15" t="s">
         <v>29</v>
@@ -2859,21 +2876,21 @@
       <c r="I42" s="17">
         <v>0</v>
       </c>
-      <c r="P42" s="23"/>
-      <c r="AL42" s="23"/>
-      <c r="BD42" s="20"/>
-      <c r="BU42" s="20"/>
-      <c r="CF42" s="20"/>
+      <c r="P42" s="21"/>
+      <c r="AL42" s="21"/>
+      <c r="BD42" s="19"/>
+      <c r="BU42" s="19"/>
+      <c r="CF42" s="19"/>
     </row>
     <row r="43" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>34</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C43" s="33" t="s">
-        <v>90</v>
+        <v>33</v>
+      </c>
+      <c r="C43" s="29" t="s">
+        <v>85</v>
       </c>
       <c r="D43" s="15" t="s">
         <v>29</v>
@@ -2889,21 +2906,21 @@
       <c r="I43" s="17">
         <v>0</v>
       </c>
-      <c r="P43" s="23"/>
-      <c r="AL43" s="23"/>
-      <c r="BD43" s="20"/>
-      <c r="BU43" s="20"/>
-      <c r="CF43" s="20"/>
+      <c r="P43" s="21"/>
+      <c r="AL43" s="21"/>
+      <c r="BD43" s="19"/>
+      <c r="BU43" s="19"/>
+      <c r="CF43" s="19"/>
     </row>
     <row r="44" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>35</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C44" s="33" t="s">
-        <v>90</v>
+        <v>34</v>
+      </c>
+      <c r="C44" s="29" t="s">
+        <v>85</v>
       </c>
       <c r="D44" s="15" t="s">
         <v>29</v>
@@ -2919,21 +2936,21 @@
       <c r="I44" s="17">
         <v>0</v>
       </c>
-      <c r="P44" s="23"/>
-      <c r="AL44" s="23"/>
-      <c r="BD44" s="20"/>
-      <c r="BU44" s="20"/>
-      <c r="CF44" s="20"/>
+      <c r="P44" s="21"/>
+      <c r="AL44" s="21"/>
+      <c r="BD44" s="19"/>
+      <c r="BU44" s="19"/>
+      <c r="CF44" s="19"/>
     </row>
     <row r="45" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>36</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C45" s="33" t="s">
-        <v>90</v>
+        <v>35</v>
+      </c>
+      <c r="C45" s="29" t="s">
+        <v>85</v>
       </c>
       <c r="D45" s="15" t="s">
         <v>29</v>
@@ -2949,21 +2966,21 @@
       <c r="I45" s="17">
         <v>0</v>
       </c>
-      <c r="P45" s="23"/>
-      <c r="AL45" s="23"/>
-      <c r="BD45" s="20"/>
-      <c r="BU45" s="20"/>
-      <c r="CF45" s="20"/>
+      <c r="P45" s="21"/>
+      <c r="AL45" s="21"/>
+      <c r="BD45" s="19"/>
+      <c r="BU45" s="19"/>
+      <c r="CF45" s="19"/>
     </row>
     <row r="46" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>37</v>
       </c>
-      <c r="B46" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="C46" s="33" t="s">
-        <v>90</v>
+      <c r="B46" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C46" s="29" t="s">
+        <v>85</v>
       </c>
       <c r="D46" s="15" t="s">
         <v>29</v>
@@ -2979,21 +2996,21 @@
       <c r="I46" s="17">
         <v>0</v>
       </c>
-      <c r="P46" s="23"/>
-      <c r="AL46" s="23"/>
-      <c r="BD46" s="20"/>
-      <c r="BU46" s="20"/>
-      <c r="CF46" s="20"/>
+      <c r="P46" s="21"/>
+      <c r="AL46" s="21"/>
+      <c r="BD46" s="19"/>
+      <c r="BU46" s="19"/>
+      <c r="CF46" s="19"/>
     </row>
     <row r="47" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>38</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C47" s="33" t="s">
-        <v>90</v>
+        <v>37</v>
+      </c>
+      <c r="C47" s="29" t="s">
+        <v>85</v>
       </c>
       <c r="D47" s="15" t="s">
         <v>29</v>
@@ -3009,21 +3026,21 @@
       <c r="I47" s="17">
         <v>0</v>
       </c>
-      <c r="P47" s="23"/>
-      <c r="AL47" s="23"/>
-      <c r="BD47" s="20"/>
-      <c r="BU47" s="20"/>
-      <c r="CF47" s="20"/>
+      <c r="P47" s="21"/>
+      <c r="AL47" s="21"/>
+      <c r="BD47" s="19"/>
+      <c r="BU47" s="19"/>
+      <c r="CF47" s="19"/>
     </row>
     <row r="48" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>39</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C48" s="33" t="s">
-        <v>90</v>
+        <v>59</v>
+      </c>
+      <c r="C48" s="29" t="s">
+        <v>85</v>
       </c>
       <c r="D48" s="15" t="s">
         <v>29</v>
@@ -3039,21 +3056,21 @@
       <c r="I48" s="17">
         <v>0</v>
       </c>
-      <c r="P48" s="23"/>
-      <c r="AL48" s="23"/>
-      <c r="BD48" s="20"/>
-      <c r="BU48" s="20"/>
-      <c r="CF48" s="20"/>
+      <c r="P48" s="21"/>
+      <c r="AL48" s="21"/>
+      <c r="BD48" s="19"/>
+      <c r="BU48" s="19"/>
+      <c r="CF48" s="19"/>
     </row>
     <row r="49" spans="1:84" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>40</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C49" s="33" t="s">
-        <v>90</v>
+        <v>38</v>
+      </c>
+      <c r="C49" s="29" t="s">
+        <v>85</v>
       </c>
       <c r="D49" s="15" t="s">
         <v>29</v>
@@ -3069,11 +3086,11 @@
       <c r="I49" s="17">
         <v>0</v>
       </c>
-      <c r="P49" s="23"/>
-      <c r="AL49" s="23"/>
-      <c r="BD49" s="20"/>
-      <c r="BU49" s="20"/>
-      <c r="CF49" s="20"/>
+      <c r="P49" s="21"/>
+      <c r="AL49" s="21"/>
+      <c r="BD49" s="19"/>
+      <c r="BU49" s="19"/>
+      <c r="CF49" s="19"/>
     </row>
     <row r="50" spans="1:84" x14ac:dyDescent="0.25">
       <c r="P50" s="1" t="s">
@@ -3185,1057 +3202,1057 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
     </row>
     <row r="2" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="26"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
     </row>
     <row r="3" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="26"/>
-      <c r="T3" s="26"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
     </row>
     <row r="4" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="26"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
     </row>
     <row r="5" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
-      <c r="T5" s="26"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
     </row>
     <row r="6" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="31"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="26"/>
-      <c r="R6" s="26"/>
-      <c r="S6" s="26"/>
-      <c r="T6" s="26"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="23"/>
     </row>
     <row r="7" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="26"/>
-      <c r="R7" s="26"/>
-      <c r="S7" s="26"/>
-      <c r="T7" s="26"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
     </row>
     <row r="8" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="26"/>
-      <c r="R8" s="26"/>
-      <c r="S8" s="26"/>
-      <c r="T8" s="26"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="23"/>
     </row>
     <row r="9" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
-      <c r="Q9" s="26"/>
-      <c r="R9" s="26"/>
-      <c r="S9" s="26"/>
-      <c r="T9" s="26"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="23"/>
     </row>
     <row r="10" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
-      <c r="P10" s="26"/>
-      <c r="Q10" s="26"/>
-      <c r="R10" s="26"/>
-      <c r="S10" s="26"/>
-      <c r="T10" s="26"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="23"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="23"/>
     </row>
     <row r="11" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="31"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="26"/>
-      <c r="R11" s="26"/>
-      <c r="S11" s="26"/>
-      <c r="T11" s="26"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23"/>
     </row>
     <row r="12" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="26"/>
-      <c r="R12" s="26"/>
-      <c r="S12" s="26"/>
-      <c r="T12" s="26"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="23"/>
     </row>
     <row r="13" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="31"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
-      <c r="P13" s="26"/>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="26"/>
-      <c r="S13" s="26"/>
-      <c r="T13" s="26"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="23"/>
+      <c r="S13" s="23"/>
+      <c r="T13" s="23"/>
     </row>
     <row r="14" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="31"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
-      <c r="Q14" s="26"/>
-      <c r="R14" s="26"/>
-      <c r="S14" s="26"/>
-      <c r="T14" s="26"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="23"/>
+      <c r="S14" s="23"/>
+      <c r="T14" s="23"/>
     </row>
     <row r="15" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="31"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="26"/>
-      <c r="O15" s="26"/>
-      <c r="P15" s="26"/>
-      <c r="Q15" s="26"/>
-      <c r="R15" s="26"/>
-      <c r="S15" s="26"/>
-      <c r="T15" s="26"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
     </row>
     <row r="16" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="31"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
-      <c r="P16" s="26"/>
-      <c r="Q16" s="26"/>
-      <c r="R16" s="26"/>
-      <c r="S16" s="26"/>
-      <c r="T16" s="26"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="23"/>
     </row>
     <row r="17" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="31"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
-      <c r="Q17" s="26"/>
-      <c r="R17" s="26"/>
-      <c r="S17" s="26"/>
-      <c r="T17" s="26"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="23"/>
+      <c r="S17" s="23"/>
+      <c r="T17" s="23"/>
     </row>
     <row r="18" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="26"/>
-      <c r="N18" s="26"/>
-      <c r="O18" s="26"/>
-      <c r="P18" s="26"/>
-      <c r="Q18" s="26"/>
-      <c r="R18" s="26"/>
-      <c r="S18" s="26"/>
-      <c r="T18" s="26"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="23"/>
+      <c r="R18" s="23"/>
+      <c r="S18" s="23"/>
+      <c r="T18" s="23"/>
     </row>
     <row r="19" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
-      <c r="P19" s="26"/>
-      <c r="Q19" s="26"/>
-      <c r="R19" s="26"/>
-      <c r="S19" s="26"/>
-      <c r="T19" s="26"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="23"/>
     </row>
     <row r="20" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="30" t="s">
+      <c r="C20" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="30" t="s">
+      <c r="E20" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26"/>
-      <c r="M20" s="26"/>
-      <c r="N20" s="26"/>
-      <c r="O20" s="26"/>
-      <c r="P20" s="26"/>
-      <c r="Q20" s="26"/>
-      <c r="R20" s="26"/>
-      <c r="S20" s="26"/>
-      <c r="T20" s="26"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="23"/>
+      <c r="S20" s="23"/>
+      <c r="T20" s="23"/>
     </row>
     <row r="21" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="31"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="26"/>
-      <c r="O21" s="26"/>
-      <c r="P21" s="26"/>
-      <c r="Q21" s="26"/>
-      <c r="R21" s="26"/>
-      <c r="S21" s="26"/>
-      <c r="T21" s="26"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="23"/>
+      <c r="P21" s="23"/>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="23"/>
+      <c r="S21" s="23"/>
+      <c r="T21" s="23"/>
     </row>
     <row r="22" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="31"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="26"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="26"/>
-      <c r="Q22" s="26"/>
-      <c r="R22" s="26"/>
-      <c r="S22" s="26"/>
-      <c r="T22" s="26"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="23"/>
+      <c r="Q22" s="23"/>
+      <c r="R22" s="23"/>
+      <c r="S22" s="23"/>
+      <c r="T22" s="23"/>
     </row>
     <row r="23" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="31"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="26"/>
-      <c r="O23" s="26"/>
-      <c r="P23" s="26"/>
-      <c r="Q23" s="26"/>
-      <c r="R23" s="26"/>
-      <c r="S23" s="26"/>
-      <c r="T23" s="26"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="23"/>
+      <c r="Q23" s="23"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="23"/>
+      <c r="T23" s="23"/>
     </row>
     <row r="24" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
-      <c r="Q24" s="26"/>
-      <c r="R24" s="26"/>
-      <c r="S24" s="26"/>
-      <c r="T24" s="26"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="23"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="23"/>
+      <c r="S24" s="23"/>
+      <c r="T24" s="23"/>
     </row>
     <row r="25" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="31"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="26"/>
-      <c r="N25" s="26"/>
-      <c r="O25" s="26"/>
-      <c r="P25" s="26"/>
-      <c r="Q25" s="26"/>
-      <c r="R25" s="26"/>
-      <c r="S25" s="26"/>
-      <c r="T25" s="26"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="23"/>
+      <c r="Q25" s="23"/>
+      <c r="R25" s="23"/>
+      <c r="S25" s="23"/>
+      <c r="T25" s="23"/>
     </row>
     <row r="26" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="31"/>
-      <c r="B26" s="31"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="26"/>
-      <c r="M26" s="26"/>
-      <c r="N26" s="26"/>
-      <c r="O26" s="26"/>
-      <c r="P26" s="26"/>
-      <c r="Q26" s="26"/>
-      <c r="R26" s="26"/>
-      <c r="S26" s="26"/>
-      <c r="T26" s="26"/>
+      <c r="A26" s="27"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="23"/>
+      <c r="Q26" s="23"/>
+      <c r="R26" s="23"/>
+      <c r="S26" s="23"/>
+      <c r="T26" s="23"/>
     </row>
     <row r="27" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="31"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="26"/>
-      <c r="M27" s="26"/>
-      <c r="N27" s="26"/>
-      <c r="O27" s="26"/>
-      <c r="P27" s="26"/>
-      <c r="Q27" s="26"/>
-      <c r="R27" s="26"/>
-      <c r="S27" s="26"/>
-      <c r="T27" s="26"/>
+      <c r="A27" s="27"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23"/>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="23"/>
+      <c r="S27" s="23"/>
+      <c r="T27" s="23"/>
     </row>
     <row r="28" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="31"/>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
-      <c r="M28" s="26"/>
-      <c r="N28" s="26"/>
-      <c r="O28" s="26"/>
-      <c r="P28" s="26"/>
-      <c r="Q28" s="26"/>
-      <c r="R28" s="26"/>
-      <c r="S28" s="26"/>
-      <c r="T28" s="26"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="23"/>
+      <c r="R28" s="23"/>
+      <c r="S28" s="23"/>
+      <c r="T28" s="23"/>
     </row>
     <row r="29" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="31"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="26"/>
-      <c r="L29" s="26"/>
-      <c r="M29" s="26"/>
-      <c r="N29" s="26"/>
-      <c r="O29" s="26"/>
-      <c r="P29" s="26"/>
-      <c r="Q29" s="26"/>
-      <c r="R29" s="26"/>
-      <c r="S29" s="26"/>
-      <c r="T29" s="26"/>
+      <c r="A29" s="27"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="23"/>
+      <c r="R29" s="23"/>
+      <c r="S29" s="23"/>
+      <c r="T29" s="23"/>
     </row>
     <row r="30" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="31"/>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="26"/>
-      <c r="L30" s="26"/>
-      <c r="M30" s="26"/>
-      <c r="N30" s="26"/>
-      <c r="O30" s="26"/>
-      <c r="P30" s="26"/>
-      <c r="Q30" s="26"/>
-      <c r="R30" s="26"/>
-      <c r="S30" s="26"/>
-      <c r="T30" s="26"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="23"/>
+      <c r="N30" s="23"/>
+      <c r="O30" s="23"/>
+      <c r="P30" s="23"/>
+      <c r="Q30" s="23"/>
+      <c r="R30" s="23"/>
+      <c r="S30" s="23"/>
+      <c r="T30" s="23"/>
     </row>
     <row r="31" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="31"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="26"/>
-      <c r="N31" s="26"/>
-      <c r="O31" s="26"/>
-      <c r="P31" s="26"/>
-      <c r="Q31" s="26"/>
-      <c r="R31" s="26"/>
-      <c r="S31" s="26"/>
-      <c r="T31" s="26"/>
+      <c r="A31" s="27"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="23"/>
+      <c r="K31" s="23"/>
+      <c r="L31" s="23"/>
+      <c r="M31" s="23"/>
+      <c r="N31" s="23"/>
+      <c r="O31" s="23"/>
+      <c r="P31" s="23"/>
+      <c r="Q31" s="23"/>
+      <c r="R31" s="23"/>
+      <c r="S31" s="23"/>
+      <c r="T31" s="23"/>
     </row>
     <row r="32" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="31"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="26"/>
-      <c r="L32" s="26"/>
-      <c r="M32" s="26"/>
-      <c r="N32" s="26"/>
-      <c r="O32" s="26"/>
-      <c r="P32" s="26"/>
-      <c r="Q32" s="26"/>
-      <c r="R32" s="26"/>
-      <c r="S32" s="26"/>
-      <c r="T32" s="26"/>
+      <c r="A32" s="27"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="23"/>
+      <c r="N32" s="23"/>
+      <c r="O32" s="23"/>
+      <c r="P32" s="23"/>
+      <c r="Q32" s="23"/>
+      <c r="R32" s="23"/>
+      <c r="S32" s="23"/>
+      <c r="T32" s="23"/>
     </row>
     <row r="33" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="31"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="26"/>
-      <c r="K33" s="26"/>
-      <c r="L33" s="26"/>
-      <c r="M33" s="26"/>
-      <c r="N33" s="26"/>
-      <c r="O33" s="26"/>
-      <c r="P33" s="26"/>
-      <c r="Q33" s="26"/>
-      <c r="R33" s="26"/>
-      <c r="S33" s="26"/>
-      <c r="T33" s="26"/>
+      <c r="A33" s="27"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="23"/>
+      <c r="M33" s="23"/>
+      <c r="N33" s="23"/>
+      <c r="O33" s="23"/>
+      <c r="P33" s="23"/>
+      <c r="Q33" s="23"/>
+      <c r="R33" s="23"/>
+      <c r="S33" s="23"/>
+      <c r="T33" s="23"/>
     </row>
     <row r="34" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="31"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="26"/>
-      <c r="K34" s="26"/>
-      <c r="L34" s="26"/>
-      <c r="M34" s="26"/>
-      <c r="N34" s="26"/>
-      <c r="O34" s="26"/>
-      <c r="P34" s="26"/>
-      <c r="Q34" s="26"/>
-      <c r="R34" s="26"/>
-      <c r="S34" s="26"/>
-      <c r="T34" s="26"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="23"/>
+      <c r="L34" s="23"/>
+      <c r="M34" s="23"/>
+      <c r="N34" s="23"/>
+      <c r="O34" s="23"/>
+      <c r="P34" s="23"/>
+      <c r="Q34" s="23"/>
+      <c r="R34" s="23"/>
+      <c r="S34" s="23"/>
+      <c r="T34" s="23"/>
     </row>
     <row r="35" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="24" t="s">
+      <c r="A35" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="B35" s="24"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
     </row>
     <row r="36" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="27" t="s">
+      <c r="A36" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="27"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
     </row>
     <row r="37" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="30" t="s">
+      <c r="B37" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="30" t="s">
+      <c r="C37" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="D37" s="30" t="s">
+      <c r="D37" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E37" s="30" t="s">
+      <c r="E37" s="26" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="31"/>
-      <c r="B38" s="31"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="31"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
     </row>
     <row r="39" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="31"/>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
     </row>
     <row r="40" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="31"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
+      <c r="A40" s="27"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
     </row>
     <row r="41" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="31"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31"/>
+      <c r="A41" s="27"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
     </row>
     <row r="42" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="31"/>
-      <c r="B42" s="31"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31"/>
+      <c r="A42" s="27"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
     </row>
     <row r="43" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="31"/>
-      <c r="B43" s="31"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="31"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
     </row>
     <row r="44" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="31"/>
-      <c r="B44" s="31"/>
-      <c r="C44" s="31"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="31"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
     </row>
     <row r="45" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="31"/>
-      <c r="B45" s="31"/>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="31"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="27"/>
     </row>
     <row r="46" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="31"/>
-      <c r="B46" s="31"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="31"/>
+      <c r="A46" s="27"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="27"/>
     </row>
     <row r="47" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="31"/>
-      <c r="B47" s="31"/>
-      <c r="C47" s="31"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="31"/>
+      <c r="A47" s="27"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27"/>
     </row>
     <row r="48" spans="1:20" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="31"/>
-      <c r="B48" s="31"/>
-      <c r="C48" s="31"/>
-      <c r="D48" s="31"/>
-      <c r="E48" s="31"/>
+      <c r="A48" s="27"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="27"/>
     </row>
     <row r="49" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="31"/>
-      <c r="B49" s="31"/>
-      <c r="C49" s="31"/>
-      <c r="D49" s="31"/>
-      <c r="E49" s="31"/>
+      <c r="A49" s="27"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="27"/>
     </row>
     <row r="50" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="31"/>
-      <c r="B50" s="31"/>
-      <c r="C50" s="31"/>
-      <c r="D50" s="31"/>
-      <c r="E50" s="31"/>
+      <c r="A50" s="27"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="27"/>
     </row>
     <row r="51" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="31"/>
-      <c r="B51" s="31"/>
-      <c r="C51" s="31"/>
-      <c r="D51" s="31"/>
-      <c r="E51" s="31"/>
+      <c r="A51" s="27"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="27"/>
     </row>
     <row r="52" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="24" t="s">
+      <c r="A52" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="B52" s="24"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
+      <c r="B52" s="32"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="32"/>
     </row>
     <row r="53" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="27" t="s">
+      <c r="A53" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="B53" s="27"/>
-      <c r="C53" s="27"/>
-      <c r="D53" s="27"/>
-      <c r="E53" s="27"/>
+      <c r="B53" s="33"/>
+      <c r="C53" s="33"/>
+      <c r="D53" s="33"/>
+      <c r="E53" s="33"/>
     </row>
     <row r="54" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="30" t="s">
+      <c r="A54" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B54" s="30" t="s">
+      <c r="B54" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C54" s="30" t="s">
+      <c r="C54" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="D54" s="30" t="s">
+      <c r="D54" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E54" s="30" t="s">
+      <c r="E54" s="26" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="31"/>
-      <c r="B55" s="31"/>
-      <c r="C55" s="31"/>
-      <c r="D55" s="31"/>
-      <c r="E55" s="31"/>
+      <c r="A55" s="27"/>
+      <c r="B55" s="27"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="27"/>
     </row>
     <row r="56" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="31"/>
-      <c r="B56" s="31"/>
-      <c r="C56" s="31"/>
-      <c r="D56" s="31"/>
-      <c r="E56" s="31"/>
+      <c r="A56" s="27"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="27"/>
+      <c r="E56" s="27"/>
     </row>
     <row r="57" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="31"/>
-      <c r="B57" s="31"/>
-      <c r="C57" s="31"/>
-      <c r="D57" s="31"/>
-      <c r="E57" s="31"/>
+      <c r="A57" s="27"/>
+      <c r="B57" s="27"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="27"/>
+      <c r="E57" s="27"/>
     </row>
     <row r="58" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="31"/>
-      <c r="B58" s="31"/>
-      <c r="C58" s="31"/>
-      <c r="D58" s="31"/>
-      <c r="E58" s="31"/>
+      <c r="A58" s="27"/>
+      <c r="B58" s="27"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="27"/>
+      <c r="E58" s="27"/>
     </row>
     <row r="59" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="31"/>
-      <c r="B59" s="31"/>
-      <c r="C59" s="31"/>
-      <c r="D59" s="31"/>
-      <c r="E59" s="31"/>
+      <c r="A59" s="27"/>
+      <c r="B59" s="27"/>
+      <c r="C59" s="27"/>
+      <c r="D59" s="27"/>
+      <c r="E59" s="27"/>
     </row>
     <row r="60" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="31"/>
-      <c r="B60" s="31"/>
-      <c r="C60" s="31"/>
-      <c r="D60" s="31"/>
-      <c r="E60" s="31"/>
+      <c r="A60" s="27"/>
+      <c r="B60" s="27"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="27"/>
+      <c r="E60" s="27"/>
     </row>
     <row r="61" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="31"/>
-      <c r="B61" s="31"/>
-      <c r="C61" s="31"/>
-      <c r="D61" s="31"/>
-      <c r="E61" s="31"/>
+      <c r="A61" s="27"/>
+      <c r="B61" s="27"/>
+      <c r="C61" s="27"/>
+      <c r="D61" s="27"/>
+      <c r="E61" s="27"/>
     </row>
     <row r="62" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="31"/>
-      <c r="B62" s="31"/>
-      <c r="C62" s="31"/>
-      <c r="D62" s="31"/>
-      <c r="E62" s="31"/>
+      <c r="A62" s="27"/>
+      <c r="B62" s="27"/>
+      <c r="C62" s="27"/>
+      <c r="D62" s="27"/>
+      <c r="E62" s="27"/>
     </row>
     <row r="63" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="31"/>
-      <c r="B63" s="31"/>
-      <c r="C63" s="31"/>
-      <c r="D63" s="31"/>
-      <c r="E63" s="31"/>
+      <c r="A63" s="27"/>
+      <c r="B63" s="27"/>
+      <c r="C63" s="27"/>
+      <c r="D63" s="27"/>
+      <c r="E63" s="27"/>
     </row>
     <row r="64" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="31"/>
-      <c r="B64" s="31"/>
-      <c r="C64" s="31"/>
-      <c r="D64" s="31"/>
-      <c r="E64" s="31"/>
+      <c r="A64" s="27"/>
+      <c r="B64" s="27"/>
+      <c r="C64" s="27"/>
+      <c r="D64" s="27"/>
+      <c r="E64" s="27"/>
     </row>
     <row r="65" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="31"/>
-      <c r="B65" s="31"/>
-      <c r="C65" s="31"/>
-      <c r="D65" s="31"/>
-      <c r="E65" s="31"/>
+      <c r="A65" s="27"/>
+      <c r="B65" s="27"/>
+      <c r="C65" s="27"/>
+      <c r="D65" s="27"/>
+      <c r="E65" s="27"/>
     </row>
     <row r="66" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="31"/>
-      <c r="B66" s="31"/>
-      <c r="C66" s="31"/>
-      <c r="D66" s="31"/>
-      <c r="E66" s="31"/>
+      <c r="A66" s="27"/>
+      <c r="B66" s="27"/>
+      <c r="C66" s="27"/>
+      <c r="D66" s="27"/>
+      <c r="E66" s="27"/>
     </row>
     <row r="67" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="31"/>
-      <c r="B67" s="31"/>
-      <c r="C67" s="31"/>
-      <c r="D67" s="31"/>
-      <c r="E67" s="31"/>
+      <c r="A67" s="27"/>
+      <c r="B67" s="27"/>
+      <c r="C67" s="27"/>
+      <c r="D67" s="27"/>
+      <c r="E67" s="27"/>
     </row>
     <row r="68" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="31"/>
-      <c r="B68" s="31"/>
-      <c r="C68" s="31"/>
-      <c r="D68" s="31"/>
-      <c r="E68" s="31"/>
+      <c r="A68" s="27"/>
+      <c r="B68" s="27"/>
+      <c r="C68" s="27"/>
+      <c r="D68" s="27"/>
+      <c r="E68" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A53:E53"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
     <mergeCell ref="A18:E18"/>
     <mergeCell ref="A19:E19"/>
     <mergeCell ref="A35:E35"/>
     <mergeCell ref="A36:E36"/>
     <mergeCell ref="A52:E52"/>
-    <mergeCell ref="A53:E53"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>